<commit_message>
fix \ to /
</commit_message>
<xml_diff>
--- a/ConsoleApp2/bin/Debug/output/FlextimeSheetForm_202002_Akiyama.xlsx
+++ b/ConsoleApp2/bin/Debug/output/FlextimeSheetForm_202002_Akiyama.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>タイムシート</t>
   </si>
@@ -131,36 +131,6 @@
     <t>19</t>
   </si>
   <si>
-    <t>Akiyama</t>
-  </si>
-  <si>
-    <t>10:30</t>
-  </si>
-  <si>
-    <t>19:00</t>
-  </si>
-  <si>
-    <t>01:00</t>
-  </si>
-  <si>
-    <t>09:30</t>
-  </si>
-  <si>
-    <t>18:00</t>
-  </si>
-  <si>
-    <t>00:30</t>
-  </si>
-  <si>
-    <t>10:15</t>
-  </si>
-  <si>
-    <t>11:00</t>
-  </si>
-  <si>
-    <t>20:00</t>
-  </si>
-  <si>
     <t>18</t>
   </si>
 </sst>
@@ -181,7 +151,7 @@
     <numFmt numFmtId="226" formatCode="[h]:mm"/>
     <numFmt numFmtId="229" formatCode="[h]:mm;[Red]\-[h]:mm"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -271,13 +241,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -293,7 +256,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -540,19 +503,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -562,7 +512,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="88">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -800,9 +750,6 @@
     <xf numFmtId="20" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="13" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="17" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="20" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="18" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -812,16 +759,28 @@
     <xf numFmtId="20" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="17" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="15" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="208" applyNumberFormat="1" fontId="4" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="20" applyNumberFormat="1" fontId="15" applyFont="1" fillId="0" applyFill="1" borderId="10" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="49" applyNumberFormat="1" fontId="5" applyFont="1" fillId="0" applyFill="1" borderId="17" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" applyNumberFormat="1" fontId="15" applyFont="1" fillId="0" applyFill="1" borderId="5" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="20" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="13" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" applyNumberFormat="1" fontId="15" applyFont="1" fillId="0" applyFill="1" borderId="20" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="49" applyNumberFormat="1" fontId="6" applyFont="1" fillId="0" applyFill="1" borderId="18" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="14" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" applyNumberFormat="1" fontId="6" applyFont="1" fillId="0" applyFill="1" borderId="8" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="12" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -32837,9 +32796,7 @@
       <c r="B5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="81" t="s">
-        <v>21</v>
-      </c>
+      <c r="C5" s="80"/>
       <c r="D5" s="72"/>
       <c r="E5" s="72"/>
       <c r="F5" s="72"/>
@@ -32912,13 +32869,13 @@
         <f ref="C8:C35" t="shared" si="0">WEEKDAY(B8)</f>
         <v>7</v>
       </c>
-      <c r="D8" s="82"/>
+      <c r="D8" s="81"/>
       <c r="E8" s="51"/>
       <c r="F8" s="52"/>
-      <c r="G8" s="82"/>
+      <c r="G8" s="81"/>
       <c r="H8" s="51"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="82"/>
+      <c r="J8" s="81"/>
       <c r="K8" s="51"/>
       <c r="L8" s="52"/>
       <c r="M8" s="76" t="s">
@@ -32945,13 +32902,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D9" s="83"/>
+      <c r="D9" s="82" t="s">
+        <v>5</v>
+      </c>
       <c r="E9" s="51"/>
       <c r="F9" s="52"/>
-      <c r="G9" s="83"/>
+      <c r="G9" s="84"/>
       <c r="H9" s="51"/>
       <c r="I9" s="52"/>
-      <c r="J9" s="83"/>
+      <c r="J9" s="86"/>
       <c r="K9" s="51"/>
       <c r="L9" s="52"/>
       <c r="M9" s="76" t="s">
@@ -32978,18 +32937,14 @@
         <v>2</v>
       </c>
       <c r="D10" s="83" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E10" s="51"/>
       <c r="F10" s="52"/>
-      <c r="G10" s="83" t="s">
-        <v>23</v>
-      </c>
+      <c r="G10" s="85"/>
       <c r="H10" s="51"/>
       <c r="I10" s="52"/>
-      <c r="J10" s="83" t="s">
-        <v>24</v>
-      </c>
+      <c r="J10" s="87"/>
       <c r="K10" s="51"/>
       <c r="L10" s="52"/>
       <c r="M10" s="76">
@@ -33014,19 +32969,15 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D11" s="83" t="s">
-        <v>22</v>
+      <c r="D11" s="83">
+        <v>0</v>
       </c>
       <c r="E11" s="51"/>
       <c r="F11" s="52"/>
-      <c r="G11" s="83" t="s">
-        <v>23</v>
-      </c>
+      <c r="G11" s="85"/>
       <c r="H11" s="51"/>
       <c r="I11" s="52"/>
-      <c r="J11" s="83" t="s">
-        <v>24</v>
-      </c>
+      <c r="J11" s="87"/>
       <c r="K11" s="51"/>
       <c r="L11" s="52"/>
       <c r="M11" s="76">
@@ -33053,19 +33004,15 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D12" s="83" t="s">
-        <v>25</v>
+      <c r="D12" s="83">
+        <v>0</v>
       </c>
       <c r="E12" s="51"/>
       <c r="F12" s="52"/>
-      <c r="G12" s="83" t="s">
-        <v>26</v>
-      </c>
+      <c r="G12" s="85"/>
       <c r="H12" s="51"/>
       <c r="I12" s="52"/>
-      <c r="J12" s="83" t="s">
-        <v>27</v>
-      </c>
+      <c r="J12" s="87"/>
       <c r="K12" s="51"/>
       <c r="L12" s="52"/>
       <c r="M12" s="76">
@@ -33092,19 +33039,15 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D13" s="83" t="s">
-        <v>22</v>
+      <c r="D13" s="83">
+        <v>0</v>
       </c>
       <c r="E13" s="51"/>
       <c r="F13" s="52"/>
-      <c r="G13" s="83" t="s">
-        <v>23</v>
-      </c>
+      <c r="G13" s="85"/>
       <c r="H13" s="51"/>
       <c r="I13" s="52"/>
-      <c r="J13" s="83" t="s">
-        <v>24</v>
-      </c>
+      <c r="J13" s="87"/>
       <c r="K13" s="51"/>
       <c r="L13" s="52"/>
       <c r="M13" s="76">
@@ -33129,19 +33072,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D14" s="83" t="s">
-        <v>28</v>
+      <c r="D14" s="83">
+        <v>0</v>
       </c>
       <c r="E14" s="51"/>
       <c r="F14" s="52"/>
-      <c r="G14" s="83" t="s">
-        <v>23</v>
-      </c>
+      <c r="G14" s="85"/>
       <c r="H14" s="51"/>
       <c r="I14" s="52"/>
-      <c r="J14" s="83" t="s">
-        <v>24</v>
-      </c>
+      <c r="J14" s="87"/>
       <c r="K14" s="51"/>
       <c r="L14" s="52"/>
       <c r="M14" s="76">
@@ -33168,13 +33107,15 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D15" s="83"/>
+      <c r="D15" s="83">
+        <v>0</v>
+      </c>
       <c r="E15" s="51"/>
       <c r="F15" s="52"/>
-      <c r="G15" s="83"/>
+      <c r="G15" s="85"/>
       <c r="H15" s="51"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="83"/>
+      <c r="J15" s="87"/>
       <c r="K15" s="51"/>
       <c r="L15" s="52"/>
       <c r="M15" s="76" t="s">
@@ -33202,13 +33143,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D16" s="83"/>
+      <c r="D16" s="83" t="s">
+        <v>12</v>
+      </c>
       <c r="E16" s="51"/>
       <c r="F16" s="52"/>
-      <c r="G16" s="83"/>
+      <c r="G16" s="85"/>
       <c r="H16" s="51"/>
       <c r="I16" s="52"/>
-      <c r="J16" s="83"/>
+      <c r="J16" s="87"/>
       <c r="K16" s="51"/>
       <c r="L16" s="52"/>
       <c r="M16" s="76" t="s">
@@ -33235,18 +33178,14 @@
         <v>2</v>
       </c>
       <c r="D17" s="83" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E17" s="51"/>
       <c r="F17" s="52"/>
-      <c r="G17" s="83" t="s">
-        <v>23</v>
-      </c>
+      <c r="G17" s="85"/>
       <c r="H17" s="51"/>
       <c r="I17" s="52"/>
-      <c r="J17" s="83" t="s">
-        <v>24</v>
-      </c>
+      <c r="J17" s="87"/>
       <c r="K17" s="51"/>
       <c r="L17" s="52"/>
       <c r="M17" s="76">
@@ -33273,13 +33212,15 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D18" s="83"/>
+      <c r="D18" s="83">
+        <v>0</v>
+      </c>
       <c r="E18" s="51"/>
       <c r="F18" s="52"/>
-      <c r="G18" s="83"/>
+      <c r="G18" s="85"/>
       <c r="H18" s="51"/>
       <c r="I18" s="52"/>
-      <c r="J18" s="83"/>
+      <c r="J18" s="87"/>
       <c r="K18" s="51"/>
       <c r="L18" s="52"/>
       <c r="M18" s="76" t="s">
@@ -33309,19 +33250,15 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D19" s="83" t="s">
-        <v>22</v>
+      <c r="D19" s="83">
+        <v>0</v>
       </c>
       <c r="E19" s="51"/>
       <c r="F19" s="52"/>
-      <c r="G19" s="83" t="s">
-        <v>23</v>
-      </c>
+      <c r="G19" s="85"/>
       <c r="H19" s="51"/>
       <c r="I19" s="52"/>
-      <c r="J19" s="83" t="s">
-        <v>24</v>
-      </c>
+      <c r="J19" s="87"/>
       <c r="K19" s="51"/>
       <c r="L19" s="52"/>
       <c r="M19" s="76">
@@ -33350,19 +33287,15 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D20" s="83" t="s">
-        <v>29</v>
+      <c r="D20" s="83">
+        <v>0</v>
       </c>
       <c r="E20" s="51"/>
       <c r="F20" s="52"/>
-      <c r="G20" s="83" t="s">
-        <v>30</v>
-      </c>
+      <c r="G20" s="85"/>
       <c r="H20" s="51"/>
       <c r="I20" s="52"/>
-      <c r="J20" s="83" t="s">
-        <v>24</v>
-      </c>
+      <c r="J20" s="87"/>
       <c r="K20" s="51"/>
       <c r="L20" s="52"/>
       <c r="M20" s="76">
@@ -33389,19 +33322,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D21" s="83" t="s">
-        <v>22</v>
+      <c r="D21" s="83">
+        <v>0</v>
       </c>
       <c r="E21" s="51"/>
       <c r="F21" s="52"/>
-      <c r="G21" s="83" t="s">
-        <v>23</v>
-      </c>
+      <c r="G21" s="85"/>
       <c r="H21" s="51"/>
       <c r="I21" s="52"/>
-      <c r="J21" s="83" t="s">
-        <v>24</v>
-      </c>
+      <c r="J21" s="87"/>
       <c r="K21" s="51"/>
       <c r="L21" s="52"/>
       <c r="M21" s="76">
@@ -33428,13 +33357,15 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D22" s="83"/>
+      <c r="D22" s="83">
+        <v>0</v>
+      </c>
       <c r="E22" s="51"/>
       <c r="F22" s="52"/>
-      <c r="G22" s="83"/>
+      <c r="G22" s="85"/>
       <c r="H22" s="51"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="83"/>
+      <c r="J22" s="87"/>
       <c r="K22" s="51"/>
       <c r="L22" s="52"/>
       <c r="M22" s="76" t="s">
@@ -33460,13 +33391,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D23" s="83"/>
+      <c r="D23" s="83" t="s">
+        <v>12</v>
+      </c>
       <c r="E23" s="51"/>
       <c r="F23" s="52"/>
-      <c r="G23" s="83"/>
+      <c r="G23" s="85"/>
       <c r="H23" s="51"/>
       <c r="I23" s="52"/>
-      <c r="J23" s="83"/>
+      <c r="J23" s="87"/>
       <c r="K23" s="51"/>
       <c r="L23" s="52"/>
       <c r="M23" s="76" t="s">
@@ -33495,18 +33428,14 @@
         <v>2</v>
       </c>
       <c r="D24" s="83" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E24" s="51"/>
       <c r="F24" s="52"/>
-      <c r="G24" s="83" t="s">
-        <v>23</v>
-      </c>
+      <c r="G24" s="85"/>
       <c r="H24" s="51"/>
       <c r="I24" s="52"/>
-      <c r="J24" s="83" t="s">
-        <v>24</v>
-      </c>
+      <c r="J24" s="87"/>
       <c r="K24" s="51"/>
       <c r="L24" s="52"/>
       <c r="M24" s="76">
@@ -33533,19 +33462,15 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D25" s="83" t="s">
-        <v>22</v>
+      <c r="D25" s="83">
+        <v>0</v>
       </c>
       <c r="E25" s="51"/>
       <c r="F25" s="52"/>
-      <c r="G25" s="83" t="s">
-        <v>23</v>
-      </c>
+      <c r="G25" s="85"/>
       <c r="H25" s="51"/>
       <c r="I25" s="52"/>
-      <c r="J25" s="83" t="s">
-        <v>24</v>
-      </c>
+      <c r="J25" s="87"/>
       <c r="K25" s="51"/>
       <c r="L25" s="52"/>
       <c r="M25" s="76">
@@ -33574,19 +33499,15 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D26" s="83" t="s">
-        <v>22</v>
+      <c r="D26" s="83">
+        <v>0</v>
       </c>
       <c r="E26" s="51"/>
       <c r="F26" s="52"/>
-      <c r="G26" s="83" t="s">
-        <v>23</v>
-      </c>
+      <c r="G26" s="85"/>
       <c r="H26" s="51"/>
       <c r="I26" s="52"/>
-      <c r="J26" s="83" t="s">
-        <v>24</v>
-      </c>
+      <c r="J26" s="87"/>
       <c r="K26" s="51"/>
       <c r="L26" s="52"/>
       <c r="M26" s="76">
@@ -33615,19 +33536,15 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D27" s="83" t="s">
-        <v>22</v>
+      <c r="D27" s="83">
+        <v>0</v>
       </c>
       <c r="E27" s="51"/>
       <c r="F27" s="52"/>
-      <c r="G27" s="83" t="s">
-        <v>23</v>
-      </c>
+      <c r="G27" s="85"/>
       <c r="H27" s="51"/>
       <c r="I27" s="52"/>
-      <c r="J27" s="83" t="s">
-        <v>24</v>
-      </c>
+      <c r="J27" s="87"/>
       <c r="K27" s="51"/>
       <c r="L27" s="52"/>
       <c r="M27" s="76">
@@ -33652,19 +33569,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D28" s="83" t="s">
-        <v>22</v>
+      <c r="D28" s="83">
+        <v>0</v>
       </c>
       <c r="E28" s="51"/>
       <c r="F28" s="52"/>
-      <c r="G28" s="83" t="s">
-        <v>23</v>
-      </c>
+      <c r="G28" s="85"/>
       <c r="H28" s="51"/>
       <c r="I28" s="52"/>
-      <c r="J28" s="83" t="s">
-        <v>24</v>
-      </c>
+      <c r="J28" s="87"/>
       <c r="K28" s="51"/>
       <c r="L28" s="52"/>
       <c r="M28" s="76">
@@ -33691,13 +33604,15 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D29" s="83"/>
+      <c r="D29" s="83">
+        <v>0</v>
+      </c>
       <c r="E29" s="51"/>
       <c r="F29" s="52"/>
-      <c r="G29" s="83"/>
+      <c r="G29" s="85"/>
       <c r="H29" s="51"/>
       <c r="I29" s="52"/>
-      <c r="J29" s="83"/>
+      <c r="J29" s="87"/>
       <c r="K29" s="51"/>
       <c r="L29" s="52"/>
       <c r="M29" s="76" t="s">
@@ -33721,13 +33636,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D30" s="83"/>
+      <c r="D30" s="83" t="s">
+        <v>12</v>
+      </c>
       <c r="E30" s="51"/>
       <c r="F30" s="52"/>
-      <c r="G30" s="83"/>
+      <c r="G30" s="85"/>
       <c r="H30" s="51"/>
       <c r="I30" s="52"/>
-      <c r="J30" s="83"/>
+      <c r="J30" s="87"/>
       <c r="K30" s="51"/>
       <c r="L30" s="52"/>
       <c r="M30" s="76" t="s">
@@ -33753,13 +33670,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D31" s="83"/>
+      <c r="D31" s="83" t="s">
+        <v>12</v>
+      </c>
       <c r="E31" s="51"/>
       <c r="F31" s="52"/>
-      <c r="G31" s="83"/>
+      <c r="G31" s="85"/>
       <c r="H31" s="51"/>
       <c r="I31" s="52"/>
-      <c r="J31" s="83"/>
+      <c r="J31" s="87"/>
       <c r="K31" s="51"/>
       <c r="L31" s="52"/>
       <c r="M31" s="76" t="s">
@@ -33783,19 +33702,15 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D32" s="83" t="s">
-        <v>22</v>
+      <c r="D32" s="83">
+        <v>0</v>
       </c>
       <c r="E32" s="51"/>
       <c r="F32" s="52"/>
-      <c r="G32" s="83" t="s">
-        <v>30</v>
-      </c>
+      <c r="G32" s="85"/>
       <c r="H32" s="51"/>
       <c r="I32" s="52"/>
-      <c r="J32" s="83" t="s">
-        <v>24</v>
-      </c>
+      <c r="J32" s="87"/>
       <c r="K32" s="51"/>
       <c r="L32" s="52"/>
       <c r="M32" s="76">
@@ -33820,19 +33735,15 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D33" s="83" t="s">
-        <v>22</v>
+      <c r="D33" s="83">
+        <v>0</v>
       </c>
       <c r="E33" s="51"/>
       <c r="F33" s="52"/>
-      <c r="G33" s="83" t="s">
-        <v>23</v>
-      </c>
+      <c r="G33" s="85"/>
       <c r="H33" s="51"/>
       <c r="I33" s="52"/>
-      <c r="J33" s="83" t="s">
-        <v>24</v>
-      </c>
+      <c r="J33" s="87"/>
       <c r="K33" s="51"/>
       <c r="L33" s="52"/>
       <c r="M33" s="76">
@@ -33859,19 +33770,15 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D34" s="83" t="s">
-        <v>22</v>
+      <c r="D34" s="83">
+        <v>0</v>
       </c>
       <c r="E34" s="51"/>
       <c r="F34" s="52"/>
-      <c r="G34" s="83" t="s">
-        <v>30</v>
-      </c>
+      <c r="G34" s="85"/>
       <c r="H34" s="51"/>
       <c r="I34" s="52"/>
-      <c r="J34" s="83" t="s">
-        <v>24</v>
-      </c>
+      <c r="J34" s="87"/>
       <c r="K34" s="51"/>
       <c r="L34" s="52"/>
       <c r="M34" s="76">
@@ -33898,19 +33805,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D35" s="84" t="s">
-        <v>22</v>
+      <c r="D35" s="83">
+        <v>0</v>
       </c>
       <c r="E35" s="51"/>
       <c r="F35" s="52"/>
-      <c r="G35" s="84" t="s">
-        <v>23</v>
-      </c>
+      <c r="G35" s="85"/>
       <c r="H35" s="51"/>
       <c r="I35" s="52"/>
-      <c r="J35" s="84" t="s">
-        <v>24</v>
-      </c>
+      <c r="J35" s="87"/>
       <c r="K35" s="51"/>
       <c r="L35" s="52"/>
       <c r="M35" s="76">
@@ -33935,13 +33838,15 @@
         <f>WEEKDAY(B36)</f>
         <v>7</v>
       </c>
-      <c r="D36" s="84"/>
+      <c r="D36" s="83">
+        <v>0</v>
+      </c>
       <c r="E36" s="51"/>
       <c r="F36" s="52"/>
-      <c r="G36" s="84"/>
+      <c r="G36" s="85"/>
       <c r="H36" s="51"/>
       <c r="I36" s="52"/>
-      <c r="J36" s="84"/>
+      <c r="J36" s="87"/>
       <c r="K36" s="51"/>
       <c r="L36" s="52"/>
       <c r="M36" s="76" t="s">
@@ -33965,19 +33870,15 @@
       <c r="C37" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D37" s="50" t="s">
+      <c r="D37" s="83" t="s">
         <v>12</v>
       </c>
       <c r="E37" s="51"/>
       <c r="F37" s="52"/>
-      <c r="G37" s="50" t="s">
-        <v>12</v>
-      </c>
+      <c r="G37" s="85"/>
       <c r="H37" s="51"/>
       <c r="I37" s="52"/>
-      <c r="J37" s="50" t="s">
-        <v>12</v>
-      </c>
+      <c r="J37" s="87"/>
       <c r="K37" s="51"/>
       <c r="L37" s="52"/>
       <c r="M37" s="76" t="s">
@@ -34001,26 +33902,22 @@
       <c r="C38" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D38" s="77" t="s">
+      <c r="D38" s="83" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" s="77"/>
+      <c r="F38" s="78"/>
+      <c r="G38" s="85"/>
+      <c r="H38" s="77"/>
+      <c r="I38" s="78"/>
+      <c r="J38" s="87"/>
+      <c r="K38" s="77"/>
+      <c r="L38" s="78"/>
+      <c r="M38" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="E38" s="78"/>
-      <c r="F38" s="79"/>
-      <c r="G38" s="77" t="s">
-        <v>19</v>
-      </c>
-      <c r="H38" s="78"/>
-      <c r="I38" s="79"/>
-      <c r="J38" s="77" t="s">
-        <v>19</v>
-      </c>
-      <c r="K38" s="78"/>
-      <c r="L38" s="79"/>
-      <c r="M38" s="80" t="s">
-        <v>19</v>
-      </c>
-      <c r="N38" s="78"/>
-      <c r="O38" s="79"/>
+      <c r="N38" s="77"/>
+      <c r="O38" s="78"/>
       <c r="P38" s="48"/>
       <c r="Q38" s="48"/>
       <c r="R38" s="20"/>
@@ -34033,7 +33930,7 @@
       <c r="C39" s="24"/>
       <c r="D39" s="25"/>
       <c r="E39" s="40" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="F39" s="25"/>
       <c r="G39" s="25"/>
@@ -48005,11 +47902,7 @@
     <mergeCell ref="M35:O35"/>
     <mergeCell ref="G44:I44"/>
     <mergeCell ref="M33:O33"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="G38:I38"/>
-    <mergeCell ref="J38:L38"/>
     <mergeCell ref="M38:O38"/>
-    <mergeCell ref="J37:L37"/>
     <mergeCell ref="M34:O34"/>
     <mergeCell ref="K48:L48"/>
     <mergeCell ref="M39:O39"/>
@@ -48021,8 +47914,6 @@
     <mergeCell ref="N44:O44"/>
     <mergeCell ref="P44:Q44"/>
     <mergeCell ref="M36:O36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="G37:I37"/>
     <mergeCell ref="C5:I5"/>
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="G8:I8"/>
@@ -48111,6 +48002,12 @@
     <mergeCell ref="D36:F36"/>
     <mergeCell ref="G36:I36"/>
     <mergeCell ref="J36:L36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="J37:L37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="G38:I38"/>
+    <mergeCell ref="J38:L38"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>